<commit_message>
v0.7.6 - cell merge bug fixed
</commit_message>
<xml_diff>
--- a/test/expect/simple.xlsx
+++ b/test/expect/simple.xlsx
@@ -46,22 +46,112 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left style="none"/>
       <right style="none"/>
       <top style="none"/>
       <bottom style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="ff7e6a54"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="ff7e6a54"/>
+      </top>
+      <bottom style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color rgb="ff7e6a54"/>
+      </top>
+      <bottom style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color rgb="ff7e6a54"/>
+      </right>
+      <top style="thin">
+        <color rgb="ff7e6a54"/>
+      </top>
+      <bottom style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="ff7e6a54"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color rgb="ff7e6a54"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="ff7e6a54"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="ff7e6a54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="ff7e6a54"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color rgb="ff7e6a54"/>
+      </right>
+      <top style="none"/>
+      <bottom style="thin">
+        <color rgb="ff7e6a54"/>
+      </bottom>
+    </border>
   </borders>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="2" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="2" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="3" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="5" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="6" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="7" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="8" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -393,7 +483,7 @@
   <sheetPr filterMode="0">
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
@@ -411,16 +501,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="2"/>
-      <c r="C1" t="s" s="2"/>
+      <c r="C1" t="s" s="3"/>
     </row>
     <row r="2" outlineLevel="0">
-      <c r="A2" t="s" s="2"/>
-      <c r="B2" t="s" s="2"/>
-      <c r="C2" t="s" s="2"/>
+      <c r="A2" t="s" s="4"/>
+      <c r="B2" t="s" s="0"/>
+      <c r="C2" t="s" s="5"/>
+    </row>
+    <row r="3" outlineLevel="0">
+      <c r="A3" t="s" s="6"/>
+      <c r="B3" t="s" s="7"/>
+      <c r="C3" t="s" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A1:C3"/>
   </mergeCells>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>